<commit_message>
new req: boa, wf
</commit_message>
<xml_diff>
--- a/data/Keywords_BS.XLSX
+++ b/data/Keywords_BS.XLSX
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prasingh/Prashant/Prashant/CareerBuilder/Extraction/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prasingh/Prashant/Prashant/CareerBuilder/ExtractionCode/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A571FD7F-EEFD-5248-B711-5FE621C26D11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6970A6DA-E423-C74A-BDC0-4E8CDEDFA69E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10000" yWindow="1920" windowWidth="23540" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="107">
   <si>
     <t>payroll</t>
   </si>
@@ -350,6 +350,9 @@
   </si>
   <si>
     <t>Fees</t>
+  </si>
+  <si>
+    <t>Average collected balance</t>
   </si>
 </sst>
 </file>
@@ -888,7 +891,7 @@
   <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1024,6 +1027,9 @@
       </c>
       <c r="F5" s="6" t="s">
         <v>33</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="K5" s="9" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
added 3 more banks
</commit_message>
<xml_diff>
--- a/data/Keywords_BS.XLSX
+++ b/data/Keywords_BS.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prasingh/Prashant/Prashant/CareerBuilder/ExtractionCode/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6970A6DA-E423-C74A-BDC0-4E8CDEDFA69E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08746DB6-72C8-E342-8AED-BD10EEC1F75E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10000" yWindow="1920" windowWidth="23540" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="109">
   <si>
     <t>payroll</t>
   </si>
@@ -353,6 +353,12 @@
   </si>
   <si>
     <t>Average collected balance</t>
+  </si>
+  <si>
+    <t>Dir Dep</t>
+  </si>
+  <si>
+    <t>Average Account Balance</t>
   </si>
 </sst>
 </file>
@@ -890,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1050,6 +1056,9 @@
       <c r="F6" s="9" t="s">
         <v>40</v>
       </c>
+      <c r="I6" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="K6" s="5" t="s">
         <v>103</v>
       </c>
@@ -1462,7 +1471,9 @@
       </c>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="14"/>
+      <c r="A44" s="14" t="s">
+        <v>107</v>
+      </c>
       <c r="C44" s="16" t="s">
         <v>81</v>
       </c>

</xml_diff>